<commit_message>
Changes in App.Config file
</commit_message>
<xml_diff>
--- a/KeywordDrivenFramework/TestFramework/ExcelSheet/TestData.xlsx
+++ b/KeywordDrivenFramework/TestFramework/ExcelSheet/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>TC_Id</t>
   </si>
@@ -43,18 +43,9 @@
     <t>LocatorName</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>txt_firstname</t>
-  </si>
-  <si>
     <t>xpath</t>
   </si>
   <si>
-    <t>class</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
@@ -67,9 +58,6 @@
     <t>LoginTest</t>
   </si>
   <si>
-    <t>AddToCartTest</t>
-  </si>
-  <si>
     <t>openbrowser</t>
   </si>
   <si>
@@ -88,9 +76,6 @@
     <t>username</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -101,6 +86,30 @@
   </si>
   <si>
     <t>passs</t>
+  </si>
+  <si>
+    <t>//*[@id="twotabsearchtextbox"]</t>
+  </si>
+  <si>
+    <t>txt_searchBox</t>
+  </si>
+  <si>
+    <t>btn_search</t>
+  </si>
+  <si>
+    <t>SearchItem</t>
+  </si>
+  <si>
+    <t>Nokia Mobiles</t>
+  </si>
+  <si>
+    <t>SearchMobileTest</t>
+  </si>
+  <si>
+    <t>//input[@value='Go']</t>
+  </si>
+  <si>
+    <t>click</t>
   </si>
 </sst>
 </file>
@@ -193,9 +202,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -507,25 +515,25 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B24"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -533,7 +541,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -547,27 +555,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -576,25 +584,21 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -604,10 +608,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,95 +624,100 @@
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
-        <v>2</v>
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
-        <v>2</v>
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
-        <v>2</v>
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
-        <v>2</v>
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
-        <v>23</v>
+      <c r="A10" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -718,37 +727,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
+      <c r="A1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -756,12 +765,39 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rename from CommonRepo to commonutilities
</commit_message>
<xml_diff>
--- a/KeywordDrivenFramework/TestFramework/ExcelSheet/TestData.xlsx
+++ b/KeywordDrivenFramework/TestFramework/ExcelSheet/TestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="60">
   <si>
     <t>TC_Id</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>LoginTest</t>
-  </si>
-  <si>
     <t>openbrowser</t>
   </si>
   <si>
@@ -73,21 +70,9 @@
     <t>input</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>gunjangarg14@gmail.com</t>
-  </si>
-  <si>
-    <t>passs</t>
-  </si>
-  <si>
     <t>//*[@id="twotabsearchtextbox"]</t>
   </si>
   <si>
@@ -110,13 +95,115 @@
   </si>
   <si>
     <t>click</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>test12345</t>
+  </si>
+  <si>
+    <t>test12345@yopmail.com</t>
+  </si>
+  <si>
+    <t>test@1234</t>
+  </si>
+  <si>
+    <t>RegistrationTest</t>
+  </si>
+  <si>
+    <t>To Navigate the Url</t>
+  </si>
+  <si>
+    <t>hover</t>
+  </si>
+  <si>
+    <t>To hover on Your account</t>
+  </si>
+  <si>
+    <t>hover_YourAccount</t>
+  </si>
+  <si>
+    <t>Clicking on "start here"</t>
+  </si>
+  <si>
+    <t>a_StartHere</t>
+  </si>
+  <si>
+    <t>Enter customer name</t>
+  </si>
+  <si>
+    <t>txt_Name</t>
+  </si>
+  <si>
+    <t>Enter Email</t>
+  </si>
+  <si>
+    <t>txt_Email</t>
+  </si>
+  <si>
+    <t>Enter Password</t>
+  </si>
+  <si>
+    <t>txt_Password</t>
+  </si>
+  <si>
+    <t>Enter Confirm Password</t>
+  </si>
+  <si>
+    <t>txt_ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Click on Create amazon account</t>
+  </si>
+  <si>
+    <t>btn_Continue</t>
+  </si>
+  <si>
+    <t>Click on Signout</t>
+  </si>
+  <si>
+    <t>btn_SignOut</t>
+  </si>
+  <si>
+    <t>//*[@id="nav-link-yourAccount"]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="nav-signin-tooltip"]/div/a</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ap_customer_name</t>
+  </si>
+  <si>
+    <t>ap_email</t>
+  </si>
+  <si>
+    <t>ap_password</t>
+  </si>
+  <si>
+    <t>ap_password_check</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>//*[@id="nav-item-signout-sa"]/span</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +223,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,11 +296,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -515,7 +610,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +628,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -541,7 +636,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -555,16 +650,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -584,10 +679,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -595,10 +690,98 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -608,10 +791,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,78 +829,247 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
+      <c r="F8" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
+      <c r="F9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -727,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,15 +1090,17 @@
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -754,32 +1108,44 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -787,23 +1153,26 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId1" display="gunjangarg14@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes for RegistrationTest and excel sheet
</commit_message>
<xml_diff>
--- a/KeywordDrivenFramework/TestFramework/ExcelSheet/TestData.xlsx
+++ b/KeywordDrivenFramework/TestFramework/ExcelSheet/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
   <si>
     <t>TC_Id</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>//*[@id="twotabsearchtextbox"]</t>
-  </si>
-  <si>
     <t>txt_searchBox</t>
   </si>
   <si>
@@ -106,12 +103,6 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
-    <t>test12345</t>
-  </si>
-  <si>
-    <t>test12345@yopmail.com</t>
-  </si>
-  <si>
     <t>test@1234</t>
   </si>
   <si>
@@ -127,12 +118,6 @@
     <t>To hover on Your account</t>
   </si>
   <si>
-    <t>hover_YourAccount</t>
-  </si>
-  <si>
-    <t>Clicking on "start here"</t>
-  </si>
-  <si>
     <t>a_StartHere</t>
   </si>
   <si>
@@ -160,9 +145,6 @@
     <t>txt_ConfirmPassword</t>
   </si>
   <si>
-    <t>Click on Create amazon account</t>
-  </si>
-  <si>
     <t>btn_Continue</t>
   </si>
   <si>
@@ -172,12 +154,6 @@
     <t>btn_SignOut</t>
   </si>
   <si>
-    <t>//*[@id="nav-link-yourAccount"]/span[2]</t>
-  </si>
-  <si>
-    <t>//*[@id="nav-signin-tooltip"]/div/a</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -196,7 +172,40 @@
     <t>continue</t>
   </si>
   <si>
-    <t>//*[@id="nav-item-signout-sa"]/span</t>
+    <t>//*[@id='nav-link-yourAccount']/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id='nav-signin-tooltip']/div/a</t>
+  </si>
+  <si>
+    <t>//*[@id='twotabsearchtextbox']</t>
+  </si>
+  <si>
+    <t>//*[@id='nav-item-signout-sa']</t>
+  </si>
+  <si>
+    <t>Click on Your Account</t>
+  </si>
+  <si>
+    <t>a_YourAccount</t>
+  </si>
+  <si>
+    <t>btn_CreateAmazonAccount</t>
+  </si>
+  <si>
+    <t>createAccountSubmit</t>
+  </si>
+  <si>
+    <t>Click on create amazon account</t>
+  </si>
+  <si>
+    <t>Click and continiue on Create amazon account</t>
+  </si>
+  <si>
+    <t>test123345</t>
+  </si>
+  <si>
+    <t>teast11112315@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -628,7 +637,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -636,7 +645,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -650,16 +659,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -679,10 +688,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -690,10 +699,10 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -701,7 +710,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>51</v>
@@ -712,7 +721,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
@@ -720,57 +729,57 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -778,14 +787,26 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -793,15 +814,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
@@ -829,7 +850,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -846,13 +867,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
@@ -860,53 +881,47 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
         <v>2</v>
@@ -914,19 +929,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
         <v>2</v>
@@ -934,16 +949,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
@@ -954,19 +969,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
         <v>2</v>
@@ -974,16 +989,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
         <v>2</v>
@@ -991,16 +1006,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
         <v>2</v>
@@ -1008,16 +1023,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
         <v>2</v>
@@ -1025,7 +1040,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -1036,7 +1051,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -1044,36 +1059,37 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1081,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,14 +1106,14 @@
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1108,16 +1124,16 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1128,21 +1144,21 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1153,7 +1169,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1164,7 +1180,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Email Implementation, Login TestCase
</commit_message>
<xml_diff>
--- a/KeywordDrivenFramework/TestFramework/ExcelSheet/TestData.xlsx
+++ b/KeywordDrivenFramework/TestFramework/ExcelSheet/TestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="78">
   <si>
     <t>TC_Id</t>
   </si>
@@ -88,6 +88,9 @@
     <t>SearchMobileTest</t>
   </si>
   <si>
+    <t>//input[@value='Go']</t>
+  </si>
+  <si>
     <t>click</t>
   </si>
   <si>
@@ -100,12 +103,6 @@
     <t>ConfirmPassword</t>
   </si>
   <si>
-    <t>test12345</t>
-  </si>
-  <si>
-    <t>test12345@yopmail.com</t>
-  </si>
-  <si>
     <t>test@1234</t>
   </si>
   <si>
@@ -121,12 +118,6 @@
     <t>To hover on Your account</t>
   </si>
   <si>
-    <t>hover_YourAccount</t>
-  </si>
-  <si>
-    <t>Clicking on "start here"</t>
-  </si>
-  <si>
     <t>a_StartHere</t>
   </si>
   <si>
@@ -154,9 +145,6 @@
     <t>txt_ConfirmPassword</t>
   </si>
   <si>
-    <t>Click on Create amazon account</t>
-  </si>
-  <si>
     <t>btn_Continue</t>
   </si>
   <si>
@@ -166,12 +154,6 @@
     <t>btn_SignOut</t>
   </si>
   <si>
-    <t>//*[@id="nav-link-yourAccount"]/span[2]</t>
-  </si>
-  <si>
-    <t>//*[@id="nav-signin-tooltip"]/div/a</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -190,26 +172,92 @@
     <t>continue</t>
   </si>
   <si>
-    <t>//*[@id="nav-item-signout-sa"]/span</t>
+    <t>//*[@id='nav-signin-tooltip']/div/a</t>
   </si>
   <si>
     <t>//*[@id='twotabsearchtextbox']</t>
   </si>
   <si>
-    <t>//div[@class='nav-search-submit nav-sprite']</t>
+    <t>//*[@id='nav-item-signout-sa']</t>
+  </si>
+  <si>
+    <t>Click on Your Account</t>
+  </si>
+  <si>
+    <t>a_YourAccount</t>
+  </si>
+  <si>
+    <t>btn_CreateAmazonAccount</t>
+  </si>
+  <si>
+    <t>createAccountSubmit</t>
+  </si>
+  <si>
+    <t>Click on create amazon account</t>
+  </si>
+  <si>
+    <t>Click and continiue on Create amazon account</t>
+  </si>
+  <si>
+    <t>searchMobileAndSelect</t>
+  </si>
+  <si>
+    <t>ItemName</t>
+  </si>
+  <si>
+    <t>Nokia Lumia</t>
+  </si>
+  <si>
+    <t>amazonLogin</t>
+  </si>
+  <si>
+    <t>//*[@id='nav-link-accountList']</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>LoginTest</t>
+  </si>
+  <si>
+    <t>//*[@id='signInSubmit']</t>
+  </si>
+  <si>
+    <t>btn_SignIn</t>
   </si>
   <si>
     <t>inputAndEnter</t>
   </si>
   <si>
-    <t>Mobile</t>
+    <t>verifyLogin</t>
+  </si>
+  <si>
+    <t>verifyItemAddedToCart</t>
+  </si>
+  <si>
+    <t>amazontest@gmail.com</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Gunjan</t>
+  </si>
+  <si>
+    <t>test12111@gmail.com</t>
+  </si>
+  <si>
+    <t>test@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +288,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -261,7 +316,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -297,17 +352,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -319,7 +363,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -625,7 +669,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -633,7 +677,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -646,7 +690,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -657,6 +701,14 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -668,16 +720,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -700,7 +752,7 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -711,7 +763,7 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -719,10 +771,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -730,65 +782,65 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -796,30 +848,53 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:D18"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
@@ -847,7 +922,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -864,13 +939,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
@@ -878,16 +953,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
@@ -895,16 +970,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
@@ -912,19 +987,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
         <v>2</v>
@@ -932,19 +1007,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
         <v>2</v>
@@ -952,16 +1027,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
@@ -972,19 +1047,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
         <v>2</v>
@@ -992,16 +1067,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
         <v>2</v>
@@ -1009,16 +1084,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
         <v>2</v>
@@ -1026,16 +1101,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
         <v>2</v>
@@ -1043,76 +1118,237 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
+      <c r="B28" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1120,19 +1356,22 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1140,24 +1379,33 @@
         <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1165,21 +1413,81 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1188,6 +1496,11 @@
     <hyperlink ref="D3" r:id="rId2"/>
     <hyperlink ref="E3" r:id="rId3"/>
     <hyperlink ref="F3" r:id="rId4"/>
+    <hyperlink ref="C7" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="F7" r:id="rId7" display="gunjangarg14@gmail.com"/>
+    <hyperlink ref="F11" r:id="rId8"/>
+    <hyperlink ref="E11" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>